<commit_message>
excel portf bijgewerkt, begin gemaakt met webapp voor beleggingspakket
</commit_message>
<xml_diff>
--- a/Ontwerp/Optieberekeningen/Portefeuille - Excel.xlsx
+++ b/Ontwerp/Optieberekeningen/Portefeuille - Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abakker/Pakket/ideaal-beleggen/Ontwerp/Optieberekeningen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DC2FD2-0721-8746-933C-217D9EBA8440}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E4451C-25AF-BC43-8B4F-10DBDD859F74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="960" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-660" yWindow="460" windowWidth="28800" windowHeight="15940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HuidigePositie" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
   <si>
     <t>positie</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Stuks</t>
   </si>
   <si>
-    <t>Koers aankoop</t>
-  </si>
-  <si>
     <t>Waarde</t>
   </si>
   <si>
@@ -159,13 +156,28 @@
     <t>stoploss verkoop 50 st ING bij koers kleiner dan 6,50; bestens;</t>
   </si>
   <si>
-    <t>euro</t>
-  </si>
-  <si>
     <t>limietorder terugkopen call dec ING 7.00 bij koers optie kleiner dan 26 euro</t>
   </si>
   <si>
     <t>doorlopend</t>
+  </si>
+  <si>
+    <t>21 sept 2020</t>
+  </si>
+  <si>
+    <t>Koers</t>
+  </si>
+  <si>
+    <t>uitgevoerd 21 sept</t>
+  </si>
+  <si>
+    <t>ma 21 sept</t>
+  </si>
+  <si>
+    <t>stoplimit kooporder 50 st ING bij koers hoger dan 6,24; bestens</t>
+  </si>
+  <si>
+    <t>wachten tot RSI een koopsignaal geeft dan inleggen kooporder 50 st tegen slotkoers + 10 euro.</t>
   </si>
 </sst>
 </file>
@@ -470,7 +482,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -488,6 +500,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Accent" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -820,19 +836,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="28.5" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
-    <col min="3" max="5" width="14.1640625" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" customWidth="1"/>
-    <col min="7" max="8" width="14.1640625" customWidth="1"/>
-    <col min="9" max="9" width="20.5" customWidth="1"/>
-    <col min="10" max="10" width="14.1640625" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="3" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -863,14 +879,14 @@
       </c>
       <c r="C2">
         <f>SUM('Tx ING aandelen'!D:D)</f>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="D2" s="4">
         <v>6.67</v>
       </c>
       <c r="E2" s="6">
         <f>D2*C2</f>
-        <v>333.5</v>
+        <v>0</v>
       </c>
       <c r="F2" s="7"/>
       <c r="H2" s="8"/>
@@ -888,7 +904,7 @@
       <c r="D3" s="6"/>
       <c r="E3" s="6">
         <f>SUM('Tx ING aandelen'!H:H)</f>
-        <v>-350.60005000000001</v>
+        <v>-35.69965000000002</v>
       </c>
       <c r="F3" s="7"/>
     </row>
@@ -900,7 +916,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="7">
         <f>E2+E3</f>
-        <v>-17.10005000000001</v>
+        <v>-35.69965000000002</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -918,14 +934,14 @@
       </c>
       <c r="C6">
         <f>SUM('Tx ING C 18 dec 2020 7.00'!D:D)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="4">
         <v>0.39</v>
       </c>
       <c r="E6" s="6">
         <f>100*D6*C6</f>
-        <v>-39</v>
+        <v>0</v>
       </c>
       <c r="F6" s="7"/>
       <c r="H6" t="s">
@@ -942,7 +958,7 @@
       <c r="D7" s="6"/>
       <c r="E7" s="6">
         <f>SUM('Tx ING C 18 dec 2020 7.00'!H:H)</f>
-        <v>52.15</v>
+        <v>25.299999999999997</v>
       </c>
       <c r="F7" s="7"/>
     </row>
@@ -955,7 +971,7 @@
       <c r="E8" s="11"/>
       <c r="F8" s="12">
         <f>E6+E7</f>
-        <v>13.149999999999999</v>
+        <v>25.299999999999997</v>
       </c>
       <c r="H8" t="s">
         <v>15</v>
@@ -1002,7 +1018,7 @@
       <c r="E11" s="14"/>
       <c r="F11" s="15">
         <f>SUM(E2:E10)</f>
-        <v>-3.9500500000000116</v>
+        <v>-10.399650000000022</v>
       </c>
       <c r="H11" s="6">
         <v>6.61</v>
@@ -1048,49 +1064,73 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97377BDB-6CD3-BB48-AE5B-B5D0CA2C99E7}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>39</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4">
+        <v>6.34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
         <v>40</v>
       </c>
-      <c r="C4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" t="s">
-        <v>42</v>
-      </c>
       <c r="C5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5">
-        <f>53-2-25</f>
-        <v>26</v>
-      </c>
-      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1101,19 +1141,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" customWidth="1"/>
-    <col min="3" max="4" width="14.1640625" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
-    <col min="6" max="8" width="14.1640625" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="3" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="8" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1127,27 +1167,27 @@
         <v>22</v>
       </c>
       <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>25</v>
-      </c>
-      <c r="H1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>28</v>
-      </c>
-      <c r="C2" t="s">
-        <v>29</v>
       </c>
       <c r="D2">
         <v>-1</v>
@@ -1165,6 +1205,34 @@
       <c r="H2">
         <f>-F2-G2</f>
         <v>52.15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0.26</v>
+      </c>
+      <c r="F3">
+        <f>E3*D3*100</f>
+        <v>26</v>
+      </c>
+      <c r="G3">
+        <v>0.85</v>
+      </c>
+      <c r="H3">
+        <f>-F3-G3</f>
+        <v>-26.85</v>
       </c>
     </row>
   </sheetData>
@@ -1178,20 +1246,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="2" width="14.1640625" customWidth="1"/>
-    <col min="3" max="3" width="25.1640625" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" customWidth="1"/>
-    <col min="6" max="7" width="14.1640625" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" customWidth="1"/>
+    <col min="1" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="7" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1205,27 +1273,27 @@
         <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="F1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
         <v>25</v>
-      </c>
-      <c r="H1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2">
         <v>50</v>
@@ -1233,17 +1301,46 @@
       <c r="E2">
         <v>6.97</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="6">
         <f>E2*D2</f>
         <v>348.5</v>
       </c>
       <c r="G2" s="6">
-        <f>0.0003*HuidigePositie!E2 + 2</f>
-        <v>2.10005</v>
+        <f>0.0003*ABS(F2) + 2</f>
+        <v>2.1045500000000001</v>
       </c>
       <c r="H2" s="6">
         <f>-F2-G2</f>
-        <v>-350.60005000000001</v>
+        <v>-350.60455000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3">
+        <v>-50</v>
+      </c>
+      <c r="E3">
+        <v>6.34</v>
+      </c>
+      <c r="F3" s="6">
+        <f>E3*D3</f>
+        <v>-317</v>
+      </c>
+      <c r="G3" s="6">
+        <f>0.0003*ABS(F3) + 2</f>
+        <v>2.0951</v>
+      </c>
+      <c r="H3" s="18">
+        <f>-F3-G3</f>
+        <v>314.9049</v>
       </c>
     </row>
   </sheetData>
@@ -1265,37 +1362,37 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="4" width="14.1640625" customWidth="1"/>
+    <col min="1" max="4" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
         <v>33</v>
-      </c>
-      <c r="B2" t="s">
-        <v>34</v>
       </c>
       <c r="C2">
         <v>0.85</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>36</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>